<commit_message>
update work on importing audit files from norway
-aggiunge i messaggi in caso che il dare e l'avere non coincidano
</commit_message>
<xml_diff>
--- a/Norway/saf-t/importapps_DocChange/test/testcases/Check_Accounting_Opening.xlsx
+++ b/Norway/saf-t/importapps_DocChange/test/testcases/Check_Accounting_Opening.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\P\Europe\Norway\saf-t\importapps_DocChange\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54227A35-93CB-42EF-BF44-A7BD601FF8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3B762-CDB9-4590-8B1A-24D614304557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="1035" windowWidth="28740" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-585" yWindow="720" windowWidth="28740" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -415,24 +415,12 @@
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -446,9 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -459,9 +444,6 @@
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -487,6 +469,24 @@
     <xf numFmtId="4" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -770,7 +770,7 @@
   <dimension ref="B1:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,29 +792,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="1"/>
@@ -829,1918 +829,1918 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="19" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="19"/>
-      <c r="P6" s="27" t="s">
+      <c r="O6" s="44"/>
+      <c r="P6" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="14" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="28" t="s">
+      <c r="O7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="35" t="s">
+      <c r="P7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="36" t="s">
+      <c r="Q7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="15" t="s">
+      <c r="R7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="S7" s="14" t="s">
+      <c r="S7" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6">
         <v>1250</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="9">
+      <c r="L8" s="7">
         <v>1</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="7">
         <v>12</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="15">
         <v>132500</v>
       </c>
-      <c r="O8" s="29">
+      <c r="O8" s="23">
         <v>145500</v>
       </c>
-      <c r="P8" s="37">
+      <c r="P8" s="31">
         <v>132500</v>
       </c>
-      <c r="Q8" s="38">
+      <c r="Q8" s="32">
         <v>145500</v>
       </c>
-      <c r="R8" s="3">
+      <c r="R8" s="2">
         <f>N8-P8</f>
         <v>0</v>
       </c>
-      <c r="S8" s="3">
+      <c r="S8" s="2">
         <f>O8-Q8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6">
         <v>1420</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="9">
+      <c r="L9" s="7">
         <v>1</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="7">
         <v>14</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="16">
         <v>957000</v>
       </c>
-      <c r="O9" s="30">
+      <c r="O9" s="24">
         <v>957000</v>
       </c>
-      <c r="P9" s="37">
+      <c r="P9" s="31">
         <v>957000</v>
       </c>
-      <c r="Q9" s="39">
+      <c r="Q9" s="33">
         <v>957000</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <f t="shared" ref="R9:R31" si="0">N9-P9</f>
         <v>0</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <f t="shared" ref="S9:S31" si="1">O9-Q9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6">
         <v>1440</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="7">
         <v>1</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="7">
         <v>14</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="16">
         <v>1578330</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="24">
         <v>1578330</v>
       </c>
-      <c r="P10" s="37">
+      <c r="P10" s="31">
         <v>1578330</v>
       </c>
-      <c r="Q10" s="39">
+      <c r="Q10" s="33">
         <v>1578330</v>
       </c>
-      <c r="R10" s="3">
+      <c r="R10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S10" s="3">
+      <c r="S10" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6">
         <v>1460</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="7">
         <v>1</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="7">
         <v>14</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="16">
         <v>30580</v>
       </c>
-      <c r="O11" s="30">
+      <c r="O11" s="24">
         <v>30580</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="31">
         <v>30580</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="32">
         <v>30580</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S11" s="3">
+      <c r="S11" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6">
         <v>1500</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="7">
         <v>1</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="7">
         <v>15</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="16">
         <v>15000</v>
       </c>
-      <c r="O12" s="30">
+      <c r="O12" s="24">
         <v>103700</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="31">
         <v>15000</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="32">
         <v>103700</v>
       </c>
-      <c r="R12" s="3">
+      <c r="R12" s="2">
         <f>N12-P12</f>
         <v>0</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6">
         <v>1900</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="7">
         <v>1</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="7">
         <v>19</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="16">
         <v>12000</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="24">
         <v>11367.5</v>
       </c>
-      <c r="P13" s="37">
+      <c r="P13" s="31">
         <v>12000</v>
       </c>
-      <c r="Q13" s="39">
+      <c r="Q13" s="33">
         <v>11367.5</v>
       </c>
-      <c r="R13" s="3">
+      <c r="R13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S13" s="3">
+      <c r="S13" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="16">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="12">
         <v>1920</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <v>1</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="3">
         <v>19</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="17">
         <v>370000</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="25">
         <v>724407</v>
       </c>
-      <c r="P14" s="40">
+      <c r="P14" s="34">
         <v>370000</v>
       </c>
-      <c r="Q14" s="41">
+      <c r="Q14" s="35">
         <v>670568.75</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S14" s="4">
+      <c r="S14" s="3">
         <f t="shared" si="1"/>
         <v>53838.25</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="17" t="s">
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="23">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="18">
         <f>SUM(N8:N14)</f>
         <v>3095410</v>
       </c>
-      <c r="O15" s="32">
+      <c r="O15" s="26">
         <f>SUM(O8:O14)</f>
         <v>3550884.5</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="36">
         <f>SUM(P8:P14)</f>
         <v>3095410</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="Q15" s="37">
         <f>SUM(Q8:Q14)</f>
         <v>3497046.25</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="5">
         <f>N15-P15</f>
         <v>0</v>
       </c>
-      <c r="S15" s="7">
+      <c r="S15" s="5">
         <f>O15-Q15</f>
         <v>53838.25</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
         <v>2000</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="7">
         <v>2</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="7">
         <v>20</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="16">
         <v>-225000</v>
       </c>
-      <c r="O16" s="30">
+      <c r="O16" s="24">
         <v>-225000</v>
       </c>
-      <c r="P16" s="37">
+      <c r="P16" s="31">
         <v>-225000</v>
       </c>
-      <c r="Q16" s="38">
+      <c r="Q16" s="32">
         <v>-225000</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8">
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
         <v>2400</v>
       </c>
-      <c r="K17" s="9" t="s">
+      <c r="K17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="7">
         <v>2</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="7">
         <v>24</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="16">
         <v>-175000</v>
       </c>
-      <c r="O17" s="30">
+      <c r="O17" s="24">
         <v>-212025</v>
       </c>
-      <c r="P17" s="37">
+      <c r="P17" s="31">
         <v>-175000</v>
       </c>
-      <c r="Q17" s="38">
+      <c r="Q17" s="32">
         <v>-212025</v>
       </c>
-      <c r="R17" s="3">
+      <c r="R17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S17" s="3">
+      <c r="S17" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6">
         <v>2700</v>
       </c>
-      <c r="K18" s="9" t="s">
+      <c r="K18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="7">
         <v>2</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="7">
         <v>27</v>
       </c>
-      <c r="N18" s="21">
+      <c r="N18" s="16">
         <v>-300000</v>
       </c>
-      <c r="O18" s="30">
+      <c r="O18" s="24">
         <v>-326375</v>
       </c>
-      <c r="P18" s="37">
+      <c r="P18" s="31">
         <v>-300000</v>
       </c>
-      <c r="Q18" s="39">
+      <c r="Q18" s="33">
         <v>-326375</v>
       </c>
-      <c r="R18" s="3">
+      <c r="R18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S18" s="3">
+      <c r="S18" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6">
         <v>2710</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="7">
         <v>2</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="7">
         <v>27</v>
       </c>
-      <c r="N19" s="21">
+      <c r="N19" s="16">
         <v>150000</v>
       </c>
-      <c r="O19" s="30">
+      <c r="O19" s="24">
         <v>72762.5</v>
       </c>
-      <c r="P19" s="37">
+      <c r="P19" s="31">
         <v>150000</v>
       </c>
-      <c r="Q19" s="38">
+      <c r="Q19" s="32">
         <v>72762.5</v>
       </c>
-      <c r="R19" s="3">
+      <c r="R19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S19" s="3">
+      <c r="S19" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6">
         <v>2711</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="7">
         <v>2</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="7">
         <v>27</v>
       </c>
-      <c r="N20" s="21"/>
-      <c r="O20" s="33">
-        <v>0</v>
-      </c>
-      <c r="P20" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="38">
-        <v>0</v>
-      </c>
-      <c r="R20" s="3">
+      <c r="N20" s="16"/>
+      <c r="O20" s="27">
+        <v>0</v>
+      </c>
+      <c r="P20" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="32">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S20" s="3">
+      <c r="S20" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6">
         <v>2740</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="9">
+      <c r="L21" s="7">
         <v>2</v>
       </c>
-      <c r="M21" s="9">
+      <c r="M21" s="7">
         <v>27</v>
       </c>
-      <c r="N21" s="21"/>
-      <c r="O21" s="33">
-        <v>0</v>
-      </c>
-      <c r="P21" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="38">
-        <v>0</v>
-      </c>
-      <c r="R21" s="3">
+      <c r="N21" s="16"/>
+      <c r="O21" s="27">
+        <v>0</v>
+      </c>
+      <c r="P21" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="32">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S21" s="3">
+      <c r="S21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="6" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="23">
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="18">
         <f>SUM(N16:N21)</f>
         <v>-550000</v>
       </c>
-      <c r="O22" s="32">
+      <c r="O22" s="26">
         <f>SUM(O16:O21)</f>
         <v>-690637.5</v>
       </c>
-      <c r="P22" s="42">
-        <f>SUM(P16:P21)</f>
-        <v>-550000</v>
-      </c>
-      <c r="Q22" s="43">
+      <c r="P22" s="36">
+        <f>SUM(P16,P17,P18,)</f>
+        <v>-700000</v>
+      </c>
+      <c r="Q22" s="37">
         <f>SUM(Q16:Q21)</f>
         <v>-690637.5</v>
       </c>
-      <c r="R22" s="7">
+      <c r="R22" s="5">
         <f>N22-P22</f>
-        <v>0</v>
-      </c>
-      <c r="S22" s="7">
+        <v>150000</v>
+      </c>
+      <c r="S22" s="5">
         <f>O22-Q22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6">
         <v>3000</v>
       </c>
-      <c r="K23" s="9" t="s">
+      <c r="K23" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="9">
+      <c r="L23" s="7">
         <v>4</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23" s="7">
         <v>30</v>
       </c>
-      <c r="N23" s="21"/>
-      <c r="O23" s="30">
+      <c r="N23" s="16"/>
+      <c r="O23" s="24">
         <v>-2316338</v>
       </c>
-      <c r="P23" s="37"/>
-      <c r="Q23" s="38">
+      <c r="P23" s="31"/>
+      <c r="Q23" s="32">
         <v>-2316338</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S23" s="3">
+      <c r="S23" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6">
         <v>4000</v>
       </c>
-      <c r="K24" s="9" t="s">
+      <c r="K24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="7">
         <v>3</v>
       </c>
-      <c r="M24" s="9">
+      <c r="M24" s="7">
         <v>40</v>
       </c>
-      <c r="N24" s="21"/>
-      <c r="O24" s="30">
+      <c r="N24" s="16"/>
+      <c r="O24" s="24">
         <v>186802</v>
       </c>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="38">
+      <c r="P24" s="31"/>
+      <c r="Q24" s="32">
         <v>186802</v>
       </c>
-      <c r="R24" s="3">
+      <c r="R24" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S24" s="3">
+      <c r="S24" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6">
         <v>5000</v>
       </c>
-      <c r="K25" s="9" t="s">
+      <c r="K25" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="7">
         <v>3</v>
       </c>
-      <c r="M25" s="9">
+      <c r="M25" s="7">
         <v>50</v>
       </c>
-      <c r="N25" s="21"/>
-      <c r="O25" s="30">
+      <c r="N25" s="16"/>
+      <c r="O25" s="24">
         <v>1496000</v>
       </c>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="38">
+      <c r="P25" s="31"/>
+      <c r="Q25" s="32">
         <v>1496000</v>
       </c>
-      <c r="R25" s="3">
+      <c r="R25" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S25" s="3">
+      <c r="S25" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6">
         <v>5092</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="6">
         <v>3</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="7">
         <v>50</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="38">
-        <v>0</v>
-      </c>
-      <c r="R26" s="3">
+      <c r="N26" s="16"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="31">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="32">
+        <v>0</v>
+      </c>
+      <c r="R26" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S26" s="3">
+      <c r="S26" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6">
         <v>6200</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L27" s="6">
         <v>3</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="7">
         <v>62</v>
       </c>
-      <c r="N27" s="21"/>
-      <c r="O27" s="30">
+      <c r="N27" s="16"/>
+      <c r="O27" s="24">
         <v>40000</v>
       </c>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="38">
+      <c r="P27" s="31"/>
+      <c r="Q27" s="32">
         <v>40000</v>
       </c>
-      <c r="R27" s="3">
+      <c r="R27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S27" s="3">
+      <c r="S27" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6">
         <v>6300</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="K28" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="7">
         <v>3</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="7">
         <v>63</v>
       </c>
-      <c r="N28" s="21"/>
-      <c r="O28" s="30">
+      <c r="N28" s="16"/>
+      <c r="O28" s="24">
         <v>150000</v>
       </c>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="38">
+      <c r="P28" s="31"/>
+      <c r="Q28" s="32">
         <v>150000</v>
       </c>
-      <c r="R28" s="3">
+      <c r="R28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S28" s="3">
+      <c r="S28" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6">
         <v>6400</v>
       </c>
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="7">
         <v>3</v>
       </c>
-      <c r="M29" s="9">
+      <c r="M29" s="7">
         <v>64</v>
       </c>
-      <c r="N29" s="21"/>
-      <c r="O29" s="30">
+      <c r="N29" s="16"/>
+      <c r="O29" s="24">
         <v>66000</v>
       </c>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="38">
+      <c r="P29" s="31"/>
+      <c r="Q29" s="32">
         <v>66000</v>
       </c>
-      <c r="R29" s="3">
+      <c r="R29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6">
         <v>7195</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="7">
         <v>3</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30" s="7">
         <v>71</v>
       </c>
-      <c r="N30" s="21"/>
-      <c r="O30" s="33">
+      <c r="N30" s="16"/>
+      <c r="O30" s="27">
         <v>699</v>
       </c>
-      <c r="P30" s="37"/>
-      <c r="Q30" s="38">
+      <c r="P30" s="31"/>
+      <c r="Q30" s="32">
         <v>699</v>
       </c>
-      <c r="R30" s="3">
+      <c r="R30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S30" s="3">
+      <c r="S30" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8">
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6">
         <v>7320</v>
       </c>
-      <c r="K31" s="8" t="s">
+      <c r="K31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="8">
+      <c r="L31" s="6">
         <v>3</v>
       </c>
-      <c r="M31" s="9">
+      <c r="M31" s="7">
         <v>73</v>
       </c>
-      <c r="N31" s="21"/>
-      <c r="O31" s="30">
+      <c r="N31" s="16"/>
+      <c r="O31" s="24">
         <v>62000</v>
       </c>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="38">
+      <c r="P31" s="31"/>
+      <c r="Q31" s="32">
         <v>62000</v>
       </c>
-      <c r="R31" s="3">
+      <c r="R31" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S31" s="3">
+      <c r="S31" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="6" t="s">
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="24"/>
-      <c r="O32" s="34">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="28">
         <f>SUM(O23:O31)</f>
         <v>-314837</v>
       </c>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="45">
+      <c r="P32" s="38"/>
+      <c r="Q32" s="39">
         <f>SUM(Q23:Q31)</f>
         <v>-314837</v>
       </c>
-      <c r="R32" s="18" t="s">
+      <c r="R32" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="S32" s="7">
+      <c r="S32" s="5">
         <f>O32-Q32</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="3"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8">
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6">
         <v>11000</v>
       </c>
-      <c r="K34" s="8" t="s">
+      <c r="K34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L34" s="8">
+      <c r="L34" s="6">
         <v>1</v>
       </c>
-      <c r="M34" s="9" t="s">
+      <c r="M34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N34" s="9">
+      <c r="N34" s="7">
         <v>32000</v>
       </c>
-      <c r="O34" s="9">
+      <c r="O34" s="7">
         <v>32000</v>
       </c>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="3"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="2"/>
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8">
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6">
         <v>11001</v>
       </c>
-      <c r="K35" s="8" t="s">
+      <c r="K35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="L35" s="8">
+      <c r="L35" s="6">
         <v>1</v>
       </c>
-      <c r="M35" s="9" t="s">
+      <c r="M35" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N35" s="9">
+      <c r="N35" s="7">
         <v>2000</v>
       </c>
-      <c r="O35" s="9">
+      <c r="O35" s="7">
         <v>2000</v>
       </c>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="3"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8">
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6">
         <v>11002</v>
       </c>
-      <c r="K36" s="8" t="s">
+      <c r="K36" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="7">
         <v>1</v>
       </c>
-      <c r="M36" s="9" t="s">
+      <c r="M36" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N36" s="9"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="3"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="2"/>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6">
         <v>11003</v>
       </c>
-      <c r="K37" s="8" t="s">
+      <c r="K37" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37" s="7">
         <v>1</v>
       </c>
-      <c r="M37" s="9" t="s">
+      <c r="M37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N37" s="9">
+      <c r="N37" s="7">
         <v>100</v>
       </c>
-      <c r="O37" s="8">
+      <c r="O37" s="6">
         <v>100</v>
       </c>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="3"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8">
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6">
         <v>11004</v>
       </c>
-      <c r="K38" s="8" t="s">
+      <c r="K38" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L38" s="8">
+      <c r="L38" s="6">
         <v>1</v>
       </c>
-      <c r="M38" s="9" t="s">
+      <c r="M38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N38" s="9"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="3"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="2"/>
     </row>
     <row r="39" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8">
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6">
         <v>11005</v>
       </c>
-      <c r="K39" s="8" t="s">
+      <c r="K39" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L39" s="8">
+      <c r="L39" s="6">
         <v>1</v>
       </c>
-      <c r="M39" s="9" t="s">
+      <c r="M39" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N39" s="9">
+      <c r="N39" s="7">
         <v>12700</v>
       </c>
-      <c r="O39" s="9">
+      <c r="O39" s="7">
         <v>12700</v>
       </c>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="3"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8">
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6">
         <v>21000</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="K40" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L40" s="8">
+      <c r="L40" s="6">
         <v>2</v>
       </c>
-      <c r="M40" s="9" t="s">
+      <c r="M40" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N40" s="9"/>
-      <c r="O40" s="8"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="3"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8">
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6">
         <v>21001</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="K41" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L41" s="8">
+      <c r="L41" s="6">
         <v>2</v>
       </c>
-      <c r="M41" s="9" t="s">
+      <c r="M41" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N41" s="9">
+      <c r="N41" s="7">
         <v>-6200</v>
       </c>
-      <c r="O41" s="9">
+      <c r="O41" s="7">
         <v>-6200</v>
       </c>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="3"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8">
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6">
         <v>21002</v>
       </c>
-      <c r="K42" s="8" t="s">
+      <c r="K42" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L42" s="8">
+      <c r="L42" s="6">
         <v>2</v>
       </c>
-      <c r="M42" s="9" t="s">
+      <c r="M42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N42" s="9"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="3"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="2"/>
     </row>
     <row r="43" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8">
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6">
         <v>21003</v>
       </c>
-      <c r="K43" s="8" t="s">
+      <c r="K43" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L43" s="8">
+      <c r="L43" s="6">
         <v>2</v>
       </c>
-      <c r="M43" s="9" t="s">
+      <c r="M43" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N43" s="9">
+      <c r="N43" s="7">
         <v>-24000</v>
       </c>
-      <c r="O43" s="9">
+      <c r="O43" s="7">
         <v>-24000</v>
       </c>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="3"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6">
         <v>21004</v>
       </c>
-      <c r="K44" s="8" t="s">
+      <c r="K44" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L44" s="8">
+      <c r="L44" s="6">
         <v>2</v>
       </c>
-      <c r="M44" s="9" t="s">
+      <c r="M44" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N44" s="9">
+      <c r="N44" s="7">
         <v>5000.5</v>
       </c>
-      <c r="O44" s="9">
+      <c r="O44" s="7">
         <v>5000.5</v>
       </c>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="3"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6">
         <v>21005</v>
       </c>
-      <c r="K45" s="8" t="s">
+      <c r="K45" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L45" s="9">
+      <c r="L45" s="7">
         <v>2</v>
       </c>
-      <c r="M45" s="9" t="s">
+      <c r="M45" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N45" s="9"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
     </row>
     <row r="46" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="10" t="s">
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="O48" s="10"/>
-      <c r="P48" s="11" t="s">
+      <c r="O48" s="41"/>
+      <c r="P48" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="Q48" s="11"/>
+      <c r="Q48" s="42"/>
     </row>
     <row r="49" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="12" t="s">
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I49" s="12" t="s">
+      <c r="I49" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="J49" s="12" t="s">
+      <c r="J49" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K49" s="12" t="s">
+      <c r="K49" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L49" s="12" t="s">
+      <c r="L49" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M49" s="13" t="s">
+      <c r="M49" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N49" s="13" t="s">
+      <c r="N49" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O49" s="12" t="s">
+      <c r="O49" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P49" s="14" t="s">
+      <c r="P49" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q49" s="14" t="s">
+      <c r="Q49" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="50" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8">
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6">
         <v>1925</v>
       </c>
-      <c r="K50" s="8" t="s">
+      <c r="K50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="L50" s="8">
+      <c r="L50" s="6">
         <v>1</v>
       </c>
-      <c r="M50" s="9">
+      <c r="M50" s="7">
         <v>19</v>
       </c>
-      <c r="N50" s="9">
+      <c r="N50" s="7">
         <v>1234.56</v>
       </c>
-      <c r="O50" s="9">
+      <c r="O50" s="7">
         <v>-11265.44</v>
       </c>
-      <c r="P50" s="9">
+      <c r="P50" s="7">
         <v>1234.56</v>
       </c>
-      <c r="Q50" s="9">
+      <c r="Q50" s="7">
         <v>12345.67</v>
       </c>
     </row>
     <row r="51" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8">
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6">
         <v>2400</v>
       </c>
-      <c r="K51" s="8" t="s">
+      <c r="K51" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L51" s="9">
+      <c r="L51" s="7">
         <v>2</v>
       </c>
-      <c r="M51" s="9">
+      <c r="M51" s="7">
         <v>24</v>
       </c>
-      <c r="N51" s="9">
+      <c r="N51" s="7">
         <v>-1234.56</v>
       </c>
-      <c r="O51" s="9">
+      <c r="O51" s="7">
         <v>-1234.56</v>
       </c>
-      <c r="P51" s="9">
+      <c r="P51" s="7">
         <v>1234.56</v>
       </c>
-      <c r="Q51" s="9">
+      <c r="Q51" s="7">
         <v>12345.67</v>
       </c>
     </row>
     <row r="52" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8">
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6">
         <v>2740</v>
       </c>
-      <c r="K52" s="8" t="s">
+      <c r="K52" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L52" s="9">
+      <c r="L52" s="7">
         <v>2</v>
       </c>
-      <c r="M52" s="9">
+      <c r="M52" s="7">
         <v>27</v>
       </c>
-      <c r="N52" s="9">
+      <c r="N52" s="7">
         <v>-1234.56</v>
       </c>
-      <c r="O52" s="9">
+      <c r="O52" s="7">
         <v>1265.44</v>
       </c>
-      <c r="P52" s="8"/>
+      <c r="P52" s="6"/>
     </row>
     <row r="53" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8">
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6">
         <v>4000</v>
       </c>
-      <c r="K53" s="9" t="s">
+      <c r="K53" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L53" s="9">
+      <c r="L53" s="7">
         <v>3</v>
       </c>
-      <c r="M53" s="9">
+      <c r="M53" s="7">
         <v>43</v>
       </c>
-      <c r="N53" s="9"/>
-      <c r="O53" s="9">
+      <c r="N53" s="7"/>
+      <c r="O53" s="7">
         <v>10000</v>
       </c>
-      <c r="P53" s="8"/>
+      <c r="P53" s="6"/>
     </row>
     <row r="54" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8">
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6">
         <v>12000</v>
       </c>
-      <c r="K54" s="9" t="s">
+      <c r="K54" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L54" s="9">
+      <c r="L54" s="7">
         <v>1</v>
       </c>
-      <c r="M54" s="9" t="s">
+      <c r="M54" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N54" s="9">
+      <c r="N54" s="7">
         <v>1234.56</v>
       </c>
-      <c r="O54" s="9">
+      <c r="O54" s="7">
         <v>1234.56</v>
       </c>
-      <c r="P54" s="8"/>
+      <c r="P54" s="6"/>
     </row>
     <row r="55" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8">
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6">
         <v>20000</v>
       </c>
-      <c r="K55" s="9" t="s">
+      <c r="K55" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L55" s="9">
+      <c r="L55" s="7">
         <v>2</v>
       </c>
-      <c r="M55" s="9" t="s">
+      <c r="M55" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N55" s="9">
+      <c r="N55" s="7">
         <v>-1234.56</v>
       </c>
-      <c r="O55" s="9">
+      <c r="O55" s="7">
         <v>-1234.56</v>
       </c>
-      <c r="P55" s="8"/>
+      <c r="P55" s="6"/>
     </row>
     <row r="56" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="9"/>
-      <c r="N56" s="9"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="8"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="6"/>
     </row>
     <row r="57" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="8"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
     </row>
     <row r="58" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="9"/>
-      <c r="N58" s="9"/>
-      <c r="O58" s="8"/>
-      <c r="P58" s="8"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="6"/>
+      <c r="P58" s="6"/>
     </row>
     <row r="59" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
-      <c r="O59" s="8"/>
-      <c r="P59" s="8"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
     </row>
     <row r="60" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="6"/>
     </row>
     <row r="61" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
-      <c r="M61" s="9"/>
-      <c r="N61" s="9"/>
-      <c r="O61" s="8"/>
-      <c r="P61" s="8"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="6"/>
+      <c r="P61" s="6"/>
     </row>
     <row r="62" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="8"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="6"/>
+      <c r="P62" s="6"/>
     </row>
     <row r="63" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="9"/>
-      <c r="N63" s="9"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="8"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="6"/>
     </row>
     <row r="64" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
-      <c r="N64" s="9"/>
-      <c r="O64" s="8"/>
-      <c r="P64" s="8"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
     </row>
     <row r="65" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="9"/>
-      <c r="L65" s="9"/>
-      <c r="M65" s="9"/>
-      <c r="N65" s="9"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="8"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="6"/>
     </row>
     <row r="66" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="8"/>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
-      <c r="O66" s="8"/>
-      <c r="P66" s="8"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="6"/>
     </row>
     <row r="67" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
-      <c r="O67" s="8"/>
-      <c r="P67" s="8"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
     </row>
     <row r="68" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
-      <c r="O68" s="8"/>
-      <c r="P68" s="8"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
     </row>
     <row r="69" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="8"/>
-      <c r="P69" s="8"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
     </row>
     <row r="70" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="9"/>
-      <c r="M70" s="9"/>
-      <c r="N70" s="9"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="8"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
     </row>
     <row r="71" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="9"/>
-      <c r="N71" s="9"/>
-      <c r="O71" s="8"/>
-      <c r="P71" s="8"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
     </row>
     <row r="72" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="8"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="6"/>
+      <c r="P72" s="6"/>
     </row>
     <row r="73" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="9"/>
-      <c r="M73" s="9"/>
-      <c r="N73" s="9"/>
-      <c r="O73" s="8"/>
-      <c r="P73" s="8"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="6"/>
+      <c r="P73" s="6"/>
     </row>
     <row r="74" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="9"/>
-      <c r="O74" s="8"/>
-      <c r="P74" s="8"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="6"/>
+      <c r="P74" s="6"/>
     </row>
     <row r="75" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="8"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="8"/>
-      <c r="P75" s="8"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="6"/>
+      <c r="P75" s="6"/>
     </row>
     <row r="76" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="8"/>
-      <c r="L76" s="8"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="9"/>
-      <c r="O76" s="8"/>
-      <c r="P76" s="8"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="7"/>
+      <c r="O76" s="6"/>
+      <c r="P76" s="6"/>
     </row>
     <row r="77" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="8"/>
-      <c r="P77" s="8"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="6"/>
+      <c r="P77" s="6"/>
     </row>
     <row r="78" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
-      <c r="I78" s="8"/>
-      <c r="J78" s="8"/>
-      <c r="K78" s="8"/>
-      <c r="L78" s="8"/>
-      <c r="M78" s="8"/>
-      <c r="N78" s="8"/>
-      <c r="O78" s="8"/>
-      <c r="P78" s="8"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
     </row>
     <row r="79" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="8"/>
-      <c r="M79" s="8"/>
-      <c r="N79" s="8"/>
-      <c r="O79" s="8"/>
-      <c r="P79" s="8"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
     </row>
     <row r="80" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="8"/>
-      <c r="M80" s="8"/>
-      <c r="N80" s="8"/>
-      <c r="O80" s="8"/>
-      <c r="P80" s="8"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+      <c r="O80" s="6"/>
+      <c r="P80" s="6"/>
     </row>
     <row r="81" spans="5:16" x14ac:dyDescent="0.25">
-      <c r="E81" s="8"/>
-      <c r="F81" s="8"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
-      <c r="L81" s="8"/>
-      <c r="M81" s="8"/>
-      <c r="N81" s="8"/>
-      <c r="O81" s="8"/>
-      <c r="P81" s="8"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+      <c r="P81" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>